<commit_message>
macro indicators documentation via gifs
</commit_message>
<xml_diff>
--- a/macroecon_indicators/macro_data.xlsx
+++ b/macroecon_indicators/macro_data.xlsx
@@ -599,22 +599,22 @@
     </row>
     <row r="4" spans="1:26">
       <c r="A4" s="2">
-        <v>44197</v>
+        <v>44927</v>
       </c>
       <c r="B4">
-        <v>20990.541</v>
+        <v>22403.435</v>
       </c>
       <c r="C4">
-        <v>262.518</v>
+        <v>300.356</v>
       </c>
       <c r="D4">
-        <v>6.4</v>
+        <v>3.4</v>
       </c>
       <c r="E4">
-        <v>0.09</v>
+        <v>4.33</v>
       </c>
       <c r="F4">
-        <v>1.08</v>
+        <v>3.53</v>
       </c>
       <c r="G4">
         <v>0</v>
@@ -623,37 +623,37 @@
         <v>0</v>
       </c>
       <c r="K4">
-        <v>0.4056864672137062</v>
+        <v>0.3838777983459662</v>
       </c>
       <c r="L4">
-        <v>263.6703333333333</v>
+        <v>301.203</v>
       </c>
       <c r="M4">
         <v>0</v>
       </c>
       <c r="O4">
-        <v>-3.125</v>
+        <v>5.882352941176472</v>
       </c>
       <c r="P4">
-        <v>6.233333333333333</v>
+        <v>3.5</v>
       </c>
       <c r="Q4">
         <v>0</v>
       </c>
       <c r="S4">
-        <v>-11.11111111111111</v>
+        <v>5.542725173210172</v>
       </c>
       <c r="T4">
-        <v>0.08</v>
+        <v>4.516666666666667</v>
       </c>
       <c r="U4">
         <v>0</v>
       </c>
       <c r="W4">
-        <v>16.66666666666665</v>
+        <v>6.232294617563738</v>
       </c>
       <c r="X4">
-        <v>1.316666666666667</v>
+        <v>3.646666666666667</v>
       </c>
       <c r="Y4">
         <v>0</v>
@@ -661,22 +661,22 @@
     </row>
     <row r="5" spans="1:26">
       <c r="A5" s="2">
-        <v>44228</v>
+        <v>44958</v>
       </c>
       <c r="B5">
-        <v>20990.541</v>
+        <v>22403.435</v>
       </c>
       <c r="C5">
-        <v>263.583</v>
+        <v>301.509</v>
       </c>
       <c r="D5">
-        <v>6.2</v>
+        <v>3.6</v>
       </c>
       <c r="E5">
-        <v>0.08</v>
+        <v>4.57</v>
       </c>
       <c r="F5">
-        <v>1.26</v>
+        <v>3.75</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -685,60 +685,60 @@
         <v>0</v>
       </c>
       <c r="K5">
-        <v>0.4056864672137062</v>
+        <v>0.3838777983459662</v>
       </c>
       <c r="L5">
-        <v>263.6703333333333</v>
+        <v>301.203</v>
       </c>
       <c r="M5">
-        <v>0.4056864672137062</v>
+        <v>0.3838777983459662</v>
       </c>
       <c r="O5">
-        <v>-3.125</v>
+        <v>5.882352941176472</v>
       </c>
       <c r="P5">
-        <v>6.233333333333333</v>
+        <v>3.5</v>
       </c>
       <c r="Q5">
-        <v>-3.125</v>
+        <v>5.882352941176472</v>
       </c>
       <c r="S5">
-        <v>-11.11111111111111</v>
+        <v>5.542725173210172</v>
       </c>
       <c r="T5">
-        <v>0.08</v>
+        <v>4.516666666666667</v>
       </c>
       <c r="U5">
-        <v>-11.11111111111111</v>
+        <v>5.542725173210172</v>
       </c>
       <c r="W5">
-        <v>16.66666666666665</v>
+        <v>6.232294617563738</v>
       </c>
       <c r="X5">
-        <v>1.316666666666667</v>
+        <v>3.646666666666667</v>
       </c>
       <c r="Y5">
-        <v>16.66666666666665</v>
+        <v>6.232294617563738</v>
       </c>
     </row>
     <row r="6" spans="1:26">
       <c r="A6" s="2">
-        <v>44256</v>
+        <v>44986</v>
       </c>
       <c r="B6">
-        <v>20990.541</v>
+        <v>22403.435</v>
       </c>
       <c r="C6">
-        <v>264.91</v>
+        <v>301.744</v>
       </c>
       <c r="D6">
-        <v>6.1</v>
+        <v>3.5</v>
       </c>
       <c r="E6">
-        <v>0.07000000000000001</v>
+        <v>4.65</v>
       </c>
       <c r="F6">
-        <v>1.61</v>
+        <v>3.66</v>
       </c>
       <c r="G6">
         <v>0</v>
@@ -747,598 +747,598 @@
         <v>0</v>
       </c>
       <c r="K6">
-        <v>0.5034467321488822</v>
+        <v>0.07794128865141747</v>
       </c>
       <c r="L6">
-        <v>263.6703333333333</v>
+        <v>301.203</v>
       </c>
       <c r="M6">
-        <v>0.9111756146245487</v>
+        <v>0.4621182863002726</v>
       </c>
       <c r="O6">
-        <v>-1.612903225806461</v>
+        <v>-2.777777777777779</v>
       </c>
       <c r="P6">
-        <v>6.233333333333333</v>
+        <v>3.5</v>
       </c>
       <c r="Q6">
-        <v>-4.687500000000011</v>
+        <v>2.941176470588247</v>
       </c>
       <c r="S6">
-        <v>-12.49999999999999</v>
+        <v>1.750547045951856</v>
       </c>
       <c r="T6">
-        <v>0.08</v>
+        <v>4.516666666666667</v>
       </c>
       <c r="U6">
-        <v>-22.22222222222221</v>
+        <v>7.390300230946889</v>
       </c>
       <c r="W6">
-        <v>27.77777777777779</v>
+        <v>-2.399999999999991</v>
       </c>
       <c r="X6">
-        <v>1.316666666666667</v>
+        <v>3.646666666666667</v>
       </c>
       <c r="Y6">
-        <v>49.07407407407407</v>
+        <v>3.682719546742219</v>
       </c>
     </row>
     <row r="7" spans="1:26">
       <c r="A7" s="2">
-        <v>44287</v>
+        <v>45017</v>
       </c>
       <c r="B7">
-        <v>21309.544</v>
+        <v>22539.418</v>
       </c>
       <c r="C7">
-        <v>266.752</v>
+        <v>303.032</v>
       </c>
       <c r="D7">
-        <v>6.1</v>
+        <v>3.4</v>
       </c>
       <c r="E7">
-        <v>0.07000000000000001</v>
+        <v>4.83</v>
       </c>
       <c r="F7">
-        <v>1.64</v>
+        <v>3.46</v>
       </c>
       <c r="G7">
-        <v>1.519746441980696</v>
+        <v>0.6069738859241891</v>
       </c>
       <c r="I7">
-        <v>1.519746441980696</v>
+        <v>0.6069738859241891</v>
       </c>
       <c r="K7">
-        <v>0.6953304896002432</v>
+        <v>0.4268519009491323</v>
       </c>
       <c r="L7">
-        <v>265.0816666666666</v>
+        <v>302.095</v>
       </c>
       <c r="M7">
-        <v>1.612841786087071</v>
+        <v>0.8909427479391052</v>
       </c>
       <c r="O7">
-        <v>0</v>
+        <v>-2.857142857142858</v>
       </c>
       <c r="P7">
-        <v>6.133333333333333</v>
+        <v>3.5</v>
       </c>
       <c r="Q7">
-        <v>-4.687500000000011</v>
+        <v>0</v>
       </c>
       <c r="S7">
-        <v>0</v>
+        <v>3.870967741935472</v>
       </c>
       <c r="T7">
-        <v>0.07333333333333335</v>
+        <v>4.683333333333334</v>
       </c>
       <c r="U7">
-        <v>-22.22222222222221</v>
+        <v>11.5473441108545</v>
       </c>
       <c r="W7">
-        <v>1.863354037267073</v>
+        <v>-5.464480874316946</v>
       </c>
       <c r="X7">
-        <v>1.503333333333333</v>
+        <v>3.623333333333334</v>
       </c>
       <c r="Y7">
-        <v>51.85185185185184</v>
+        <v>-1.98300283286118</v>
       </c>
     </row>
     <row r="8" spans="1:26">
       <c r="A8" s="2">
-        <v>44317</v>
+        <v>45047</v>
       </c>
       <c r="B8">
-        <v>21309.544</v>
+        <v>22539.418</v>
       </c>
       <c r="C8">
-        <v>268.452</v>
+        <v>303.365</v>
       </c>
       <c r="D8">
-        <v>5.8</v>
+        <v>3.7</v>
       </c>
       <c r="E8">
-        <v>0.06</v>
+        <v>5.06</v>
       </c>
       <c r="F8">
-        <v>1.62</v>
+        <v>3.57</v>
       </c>
       <c r="G8">
         <v>0</v>
       </c>
       <c r="I8">
-        <v>1.519746441980696</v>
+        <v>0.6069738859241891</v>
       </c>
       <c r="K8">
-        <v>0.6372960652591075</v>
+        <v>0.109889384619466</v>
       </c>
       <c r="L8">
-        <v>266.7046666666667</v>
+        <v>302.7136666666667</v>
       </c>
       <c r="M8">
-        <v>2.260416428587764</v>
+        <v>1.001811184061596</v>
       </c>
       <c r="O8">
-        <v>-4.91803278688524</v>
+        <v>8.823529411764719</v>
       </c>
       <c r="P8">
-        <v>6</v>
+        <v>3.533333333333333</v>
       </c>
       <c r="Q8">
-        <v>-9.375000000000011</v>
+        <v>8.823529411764719</v>
       </c>
       <c r="S8">
-        <v>-14.2857142857143</v>
+        <v>4.761904761904745</v>
       </c>
       <c r="T8">
-        <v>0.06666666666666667</v>
+        <v>4.846666666666667</v>
       </c>
       <c r="U8">
-        <v>-33.33333333333334</v>
+        <v>16.85912240184757</v>
       </c>
       <c r="W8">
-        <v>-1.219512195121941</v>
+        <v>3.179190751445082</v>
       </c>
       <c r="X8">
-        <v>1.623333333333333</v>
+        <v>3.563333333333334</v>
       </c>
       <c r="Y8">
-        <v>50</v>
+        <v>1.133144475920678</v>
       </c>
     </row>
     <row r="9" spans="1:26">
       <c r="A9" s="2">
-        <v>44348</v>
+        <v>45078</v>
       </c>
       <c r="B9">
-        <v>21309.544</v>
+        <v>22539.418</v>
       </c>
       <c r="C9">
-        <v>270.664</v>
+        <v>304.003</v>
       </c>
       <c r="D9">
-        <v>5.9</v>
+        <v>3.6</v>
       </c>
       <c r="E9">
-        <v>0.08</v>
+        <v>5.08</v>
       </c>
       <c r="F9">
-        <v>1.52</v>
+        <v>3.75</v>
       </c>
       <c r="G9">
         <v>0</v>
       </c>
       <c r="I9">
-        <v>1.519746441980696</v>
+        <v>0.6069738859241891</v>
       </c>
       <c r="K9">
-        <v>0.823983430929931</v>
+        <v>0.2103077151286437</v>
       </c>
       <c r="L9">
-        <v>268.6226666666666</v>
+        <v>303.4666666666666</v>
       </c>
       <c r="M9">
-        <v>3.103025316359265</v>
+        <v>1.214225785401313</v>
       </c>
       <c r="O9">
-        <v>1.724137931034497</v>
+        <v>-2.702702702702708</v>
       </c>
       <c r="P9">
-        <v>5.933333333333333</v>
+        <v>3.566666666666666</v>
       </c>
       <c r="Q9">
-        <v>-7.8125</v>
+        <v>5.882352941176472</v>
       </c>
       <c r="S9">
-        <v>33.33333333333335</v>
+        <v>0.3952569169960674</v>
       </c>
       <c r="T9">
-        <v>0.06999999999999999</v>
+        <v>4.989999999999999</v>
       </c>
       <c r="U9">
-        <v>-11.11111111111111</v>
+        <v>17.32101616628174</v>
       </c>
       <c r="W9">
-        <v>-6.172839506172845</v>
+        <v>5.042016806722693</v>
       </c>
       <c r="X9">
-        <v>1.593333333333333</v>
+        <v>3.593333333333334</v>
       </c>
       <c r="Y9">
-        <v>40.74074074074075</v>
+        <v>6.232294617563738</v>
       </c>
     </row>
     <row r="10" spans="1:26">
       <c r="A10" s="2">
-        <v>44378</v>
+        <v>45108</v>
       </c>
       <c r="B10">
-        <v>21483.083</v>
+        <v>22780.933</v>
       </c>
       <c r="C10">
-        <v>271.994</v>
+        <v>304.628</v>
       </c>
       <c r="D10">
-        <v>5.4</v>
+        <v>3.5</v>
       </c>
       <c r="E10">
-        <v>0.1</v>
+        <v>5.12</v>
       </c>
       <c r="F10">
-        <v>1.32</v>
+        <v>3.9</v>
       </c>
       <c r="G10">
-        <v>0.814372189287571</v>
+        <v>1.071522787323076</v>
       </c>
       <c r="I10">
-        <v>2.346495023639439</v>
+        <v>1.685000536748049</v>
       </c>
       <c r="K10">
-        <v>0.4913841515680195</v>
+        <v>0.2055900764137197</v>
       </c>
       <c r="L10">
-        <v>270.37</v>
+        <v>303.9986666666666</v>
       </c>
       <c r="M10">
-        <v>3.609657242551001</v>
+        <v>1.42231218953508</v>
       </c>
       <c r="O10">
-        <v>-8.474576271186439</v>
+        <v>-2.777777777777779</v>
       </c>
       <c r="P10">
-        <v>5.7</v>
+        <v>3.6</v>
       </c>
       <c r="Q10">
-        <v>-15.625</v>
+        <v>2.941176470588247</v>
       </c>
       <c r="S10">
-        <v>25</v>
+        <v>0.7874015748031482</v>
       </c>
       <c r="T10">
-        <v>0.08</v>
+        <v>5.086666666666667</v>
       </c>
       <c r="U10">
-        <v>11.11111111111112</v>
+        <v>18.24480369515011</v>
       </c>
       <c r="W10">
-        <v>-13.1578947368421</v>
+        <v>4.000000000000004</v>
       </c>
       <c r="X10">
-        <v>1.486666666666667</v>
+        <v>3.74</v>
       </c>
       <c r="Y10">
-        <v>22.22222222222221</v>
+        <v>10.48158640226628</v>
       </c>
     </row>
     <row r="11" spans="1:26">
       <c r="A11" s="2">
-        <v>44409</v>
+        <v>45139</v>
       </c>
       <c r="B11">
-        <v>21483.083</v>
+        <v>22780.933</v>
       </c>
       <c r="C11">
-        <v>272.789</v>
+        <v>306.187</v>
       </c>
       <c r="D11">
-        <v>5.1</v>
+        <v>3.8</v>
       </c>
       <c r="E11">
-        <v>0.09</v>
+        <v>5.33</v>
       </c>
       <c r="F11">
-        <v>1.28</v>
+        <v>4.17</v>
       </c>
       <c r="G11">
         <v>0</v>
       </c>
       <c r="I11">
-        <v>2.346495023639439</v>
+        <v>1.685000536748049</v>
       </c>
       <c r="K11">
-        <v>0.2922858592468769</v>
+        <v>0.5117717347059347</v>
       </c>
       <c r="L11">
-        <v>271.8156666666667</v>
+        <v>304.9393333333333</v>
       </c>
       <c r="M11">
-        <v>3.912493619485136</v>
+        <v>1.941362916006351</v>
       </c>
       <c r="O11">
-        <v>-5.55555555555557</v>
+        <v>8.571428571428562</v>
       </c>
       <c r="P11">
-        <v>5.466666666666666</v>
+        <v>3.633333333333333</v>
       </c>
       <c r="Q11">
-        <v>-20.31250000000001</v>
+        <v>11.76470588235294</v>
       </c>
       <c r="S11">
-        <v>-10.00000000000001</v>
+        <v>4.1015625</v>
       </c>
       <c r="T11">
-        <v>0.09000000000000001</v>
+        <v>5.176666666666667</v>
       </c>
       <c r="U11">
-        <v>0</v>
+        <v>23.09468822170901</v>
       </c>
       <c r="W11">
-        <v>-3.030303030303028</v>
+        <v>6.923076923076921</v>
       </c>
       <c r="X11">
-        <v>1.373333333333333</v>
+        <v>3.94</v>
       </c>
       <c r="Y11">
-        <v>18.51851851851851</v>
+        <v>18.13031161473089</v>
       </c>
     </row>
     <row r="12" spans="1:26">
       <c r="A12" s="2">
-        <v>44440</v>
+        <v>45170</v>
       </c>
       <c r="B12">
-        <v>21483.083</v>
+        <v>22780.933</v>
       </c>
       <c r="C12">
-        <v>273.887</v>
+        <v>307.288</v>
       </c>
       <c r="D12">
-        <v>4.7</v>
+        <v>3.8</v>
       </c>
       <c r="E12">
-        <v>0.08</v>
+        <v>5.33</v>
       </c>
       <c r="F12">
-        <v>1.37</v>
+        <v>4.38</v>
       </c>
       <c r="G12">
         <v>0</v>
       </c>
       <c r="I12">
-        <v>2.346495023639439</v>
+        <v>1.685000536748049</v>
       </c>
       <c r="K12">
-        <v>0.4025088988192316</v>
+        <v>0.3595841756834917</v>
       </c>
       <c r="L12">
-        <v>272.89</v>
+        <v>306.0343333333333</v>
       </c>
       <c r="M12">
-        <v>4.33075065328854</v>
+        <v>2.307927925528386</v>
       </c>
       <c r="O12">
-        <v>-7.843137254901955</v>
+        <v>0</v>
       </c>
       <c r="P12">
-        <v>5.066666666666666</v>
+        <v>3.7</v>
       </c>
       <c r="Q12">
-        <v>-26.5625</v>
+        <v>11.76470588235294</v>
       </c>
       <c r="S12">
-        <v>-11.11111111111111</v>
+        <v>0</v>
       </c>
       <c r="T12">
-        <v>0.09000000000000001</v>
+        <v>5.26</v>
       </c>
       <c r="U12">
-        <v>-11.11111111111111</v>
+        <v>23.09468822170901</v>
       </c>
       <c r="W12">
-        <v>7.03125</v>
+        <v>5.035971223021574</v>
       </c>
       <c r="X12">
-        <v>1.323333333333333</v>
+        <v>4.149999999999999</v>
       </c>
       <c r="Y12">
-        <v>26.85185185185186</v>
+        <v>24.07932011331446</v>
       </c>
     </row>
     <row r="13" spans="1:26">
       <c r="A13" s="2">
-        <v>44470</v>
+        <v>45200</v>
       </c>
       <c r="B13">
-        <v>21847.602</v>
+        <v>22960.6</v>
       </c>
       <c r="C13">
-        <v>276.434</v>
+        <v>307.531</v>
       </c>
       <c r="D13">
-        <v>4.5</v>
+        <v>3.8</v>
       </c>
       <c r="E13">
-        <v>0.08</v>
+        <v>5.33</v>
       </c>
       <c r="F13">
-        <v>1.58</v>
+        <v>4.8</v>
       </c>
       <c r="G13">
-        <v>1.696772292878079</v>
+        <v>0.788672702737836</v>
       </c>
       <c r="I13">
-        <v>4.083081993932391</v>
+        <v>2.486962378760205</v>
       </c>
       <c r="K13">
-        <v>0.929945561490686</v>
+        <v>0.07907890968732456</v>
       </c>
       <c r="L13">
-        <v>274.37</v>
+        <v>307.002</v>
       </c>
       <c r="M13">
-        <v>5.30096983825874</v>
+        <v>2.388831919455581</v>
       </c>
       <c r="O13">
-        <v>-4.255319148936176</v>
+        <v>0</v>
       </c>
       <c r="P13">
-        <v>4.766666666666667</v>
+        <v>3.8</v>
       </c>
       <c r="Q13">
-        <v>-29.6875</v>
+        <v>11.76470588235294</v>
       </c>
       <c r="S13">
         <v>0</v>
       </c>
       <c r="T13">
-        <v>0.08333333333333333</v>
+        <v>5.33</v>
       </c>
       <c r="U13">
-        <v>-11.11111111111111</v>
+        <v>23.09468822170901</v>
       </c>
       <c r="W13">
-        <v>15.32846715328466</v>
+        <v>9.589041095890405</v>
       </c>
       <c r="X13">
-        <v>1.41</v>
+        <v>4.449999999999999</v>
       </c>
       <c r="Y13">
-        <v>46.2962962962963</v>
+        <v>35.97733711048159</v>
       </c>
     </row>
     <row r="14" spans="1:26">
       <c r="A14" s="2">
-        <v>44501</v>
+        <v>45231</v>
       </c>
       <c r="B14">
-        <v>21847.602</v>
+        <v>22960.6</v>
       </c>
       <c r="C14">
-        <v>278.799</v>
+        <v>308.024</v>
       </c>
       <c r="D14">
-        <v>4.1</v>
+        <v>3.7</v>
       </c>
       <c r="E14">
-        <v>0.08</v>
+        <v>5.33</v>
       </c>
       <c r="F14">
-        <v>1.56</v>
+        <v>4.5</v>
       </c>
       <c r="G14">
         <v>0</v>
       </c>
       <c r="I14">
-        <v>4.083081993932391</v>
+        <v>2.486962378760205</v>
       </c>
       <c r="K14">
-        <v>0.8555387542776849</v>
+        <v>0.160309042015272</v>
       </c>
       <c r="L14">
-        <v>276.3733333333333</v>
+        <v>307.6143333333333</v>
       </c>
       <c r="M14">
-        <v>6.201860443855289</v>
+        <v>2.552970475036287</v>
       </c>
       <c r="O14">
-        <v>-8.888888888888902</v>
+        <v>-2.631578947368407</v>
       </c>
       <c r="P14">
-        <v>4.433333333333334</v>
+        <v>3.766666666666667</v>
       </c>
       <c r="Q14">
-        <v>-35.93750000000001</v>
+        <v>8.823529411764719</v>
       </c>
       <c r="S14">
         <v>0</v>
       </c>
       <c r="T14">
-        <v>0.08</v>
+        <v>5.33</v>
       </c>
       <c r="U14">
-        <v>-11.11111111111111</v>
+        <v>23.09468822170901</v>
       </c>
       <c r="W14">
-        <v>-1.265822784810122</v>
+        <v>-6.25</v>
       </c>
       <c r="X14">
-        <v>1.503333333333333</v>
+        <v>4.56</v>
       </c>
       <c r="Y14">
-        <v>44.44444444444444</v>
+        <v>27.47875354107649</v>
       </c>
     </row>
     <row r="15" spans="1:26">
       <c r="A15" s="2">
-        <v>44531</v>
+        <v>45261</v>
       </c>
       <c r="B15">
-        <v>21847.602</v>
+        <v>22960.6</v>
       </c>
       <c r="C15">
-        <v>280.808</v>
+        <v>308.742</v>
       </c>
       <c r="D15">
-        <v>3.9</v>
+        <v>3.7</v>
       </c>
       <c r="E15">
-        <v>0.08</v>
+        <v>5.33</v>
       </c>
       <c r="F15">
-        <v>1.47</v>
+        <v>4.02</v>
       </c>
       <c r="G15">
         <v>0</v>
       </c>
       <c r="I15">
-        <v>4.083081993932391</v>
+        <v>2.486962378760205</v>
       </c>
       <c r="K15">
-        <v>0.7205908199096944</v>
+        <v>0.2330987195803047</v>
       </c>
       <c r="L15">
-        <v>278.6803333333333</v>
+        <v>308.099</v>
       </c>
       <c r="M15">
-        <v>6.967141300786994</v>
+        <v>2.792020136105156</v>
       </c>
       <c r="O15">
-        <v>-4.878048780487799</v>
+        <v>0</v>
       </c>
       <c r="P15">
-        <v>4.166666666666667</v>
+        <v>3.733333333333333</v>
       </c>
       <c r="Q15">
-        <v>-39.0625</v>
+        <v>8.823529411764719</v>
       </c>
       <c r="S15">
         <v>0</v>
       </c>
       <c r="T15">
-        <v>0.08</v>
+        <v>5.33</v>
       </c>
       <c r="U15">
-        <v>-11.11111111111111</v>
+        <v>23.09468822170901</v>
       </c>
       <c r="W15">
-        <v>-5.769230769230771</v>
+        <v>-10.66666666666668</v>
       </c>
       <c r="X15">
-        <v>1.536666666666666</v>
+        <v>4.44</v>
       </c>
       <c r="Y15">
-        <v>36.11111111111109</v>
+        <v>13.88101983002832</v>
       </c>
     </row>
   </sheetData>

</xml_diff>